<commit_message>
Two exercises are ready
</commit_message>
<xml_diff>
--- a/BA_04/src/ex_01_BRB_crud.xlsx
+++ b/BA_04/src/ex_01_BRB_crud.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Пользователь\Desktop\Business-and-system-analyses\BA_04\src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5E0DA1-AE0B-4FD3-95C9-6F3D845550B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2436" yWindow="3396" windowWidth="18948" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
+  <si>
+    <t>Клиенты</t>
+  </si>
+  <si>
+    <t>Ресурс</t>
+  </si>
+  <si>
+    <t>Мастер</t>
+  </si>
+  <si>
+    <t>Услуга</t>
+  </si>
+  <si>
+    <t>Статус услуги</t>
+  </si>
+  <si>
+    <t>Расписание</t>
+  </si>
   <si>
     <t>Отзывы</t>
   </si>
@@ -27,79 +51,90 @@
     <t>Сущность</t>
   </si>
   <si>
-    <t>номер</t>
-  </si>
-  <si>
-    <t>Расчеты</t>
-  </si>
-  <si>
-    <t>Пользователи</t>
-  </si>
-  <si>
-    <t>Услуги</t>
-  </si>
-  <si>
-    <t>Мастера</t>
-  </si>
-  <si>
-    <t>Расписание</t>
-  </si>
-  <si>
-    <t>Отчет об услугах</t>
-  </si>
-  <si>
-    <t>Зарегистрированный/Не зарегистрированный</t>
-  </si>
-  <si>
-    <t>Косметология/Стрижка</t>
-  </si>
-  <si>
-    <t>Косметологи/Парикмахеры</t>
-  </si>
-  <si>
-    <t>Утреннее/Буднее/Вечернее</t>
-  </si>
-  <si>
-    <t>От пользователей</t>
-  </si>
-  <si>
-    <t>Клиенты/Мастера</t>
-  </si>
-  <si>
-    <t>Косметологические/праикмахерские</t>
-  </si>
-  <si>
-    <t>Атрибуты</t>
-  </si>
-  <si>
-    <t>Назначение</t>
-  </si>
-  <si>
-    <t>Идентификация клиентов</t>
-  </si>
-  <si>
-    <t>Определения возможного набора услуг</t>
-  </si>
-  <si>
-    <t>Сопоставление мастер/услуга</t>
-  </si>
-  <si>
-    <t>Формирование рабочего дня</t>
-  </si>
-  <si>
-    <t>Отслеживание уровня сервиса</t>
-  </si>
-  <si>
-    <t>Аудит проведенных работ</t>
-  </si>
-  <si>
-    <t>Анализ для менеджерского состава</t>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Роль</t>
+  </si>
+  <si>
+    <t>Действие</t>
+  </si>
+  <si>
+    <t>Менеджер</t>
+  </si>
+  <si>
+    <t>Создает</t>
+  </si>
+  <si>
+    <t>Просматривает</t>
+  </si>
+  <si>
+    <t>Редактирует</t>
+  </si>
+  <si>
+    <t>Менеджер,
+Клиент</t>
+  </si>
+  <si>
+    <t>Менеджер, 
+Клиент</t>
+  </si>
+  <si>
+    <t>Клиент</t>
+  </si>
+  <si>
+    <t>Регистрируется</t>
+  </si>
+  <si>
+    <t>Менеджер,
+Мастер</t>
+  </si>
+  <si>
+    <t>удаляет</t>
+  </si>
+  <si>
+    <t>Кладется в архив</t>
+  </si>
+  <si>
+    <t>Добавляет</t>
+  </si>
+  <si>
+    <t>Просаматривает</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Менеджер </t>
+  </si>
+  <si>
+    <t>Менеджер, 
+Мастер, 
+Клиент</t>
+  </si>
+  <si>
+    <t>Проставляет отметку</t>
+  </si>
+  <si>
+    <t>Отправляет в архив</t>
+  </si>
+  <si>
+    <t>Просамтривает</t>
+  </si>
+  <si>
+    <t>Удаляет</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -109,12 +144,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -144,9 +185,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -165,9 +217,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -205,12 +257,12 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -245,7 +297,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -277,7 +329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,133 +478,277 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
+      <c r="G9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>